<commit_message>
started adding to the gantt chart
</commit_message>
<xml_diff>
--- a/docs/TopperNav Gannt Chart.xlsx
+++ b/docs/TopperNav Gannt Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mlwat\Dropbox (Personal)\Client Folders\Microsoft\Microsoft Office Template Project\02_Template Sent for MS Review\Rapid Refresh Batch B78\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/014b0dfa241f4418/Desktop/TopperNav/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2DFD3AE-3F04-4337-B9A1-E7D51701EAA2}"/>
+  <xr:revisionPtr revIDLastSave="92" documentId="11_3C4179B01545E19DD6C385890107473B0B440F85" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13B951E4-8C72-4EE2-A6BC-44BDA3206493}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project schedule" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>TopperNav</t>
   </si>
@@ -157,6 +157,21 @@
   <si>
     <t>Businesses will find invoices, time sheets, inventory trackers, financial statements, and project planning templates. Teachers and students will find resources such as class schedules, grade books, and attendance sheets. Organize your family life with meal planners, checklists, and exercise logs. Each template is thoroughly researched, refined, and improved over time through feedback from thousands of users.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Team Creation </t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation </t>
+  </si>
+  <si>
+    <t>CATME</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research </t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +184,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ d\,\ yyyy"/>
     <numFmt numFmtId="167" formatCode="d"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,6 +1073,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1070,40 +1119,6 @@
     <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="19" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="Comma" xfId="4" builtinId="3" customBuiltin="1"/>
@@ -1121,18 +1136,6 @@
     <cellStyle name="zHiddenText" xfId="3" xr:uid="{26E66EE6-E33F-4D77-BAE4-0FB4F5BBF673}"/>
   </cellStyles>
   <dxfs count="18">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="5"/>
-        </left>
-        <right style="thin">
-          <color theme="5"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1241,6 +1244,18 @@
         <bottom style="thin">
           <color theme="0" tint="-4.9989318521683403E-2"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color theme="5"/>
+        </left>
+        <right style="thin">
+          <color theme="5"/>
+        </right>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1704,26 +1719,26 @@
   </sheetPr>
   <dimension ref="A1:BL36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A20" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B31"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="AK4" sqref="AK4:AQ4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="30" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.75" style="13" customWidth="1"/>
-    <col min="2" max="2" width="22.75" customWidth="1"/>
-    <col min="3" max="3" width="16.75" customWidth="1"/>
-    <col min="4" max="4" width="10.75" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.75" customWidth="1"/>
-    <col min="7" max="7" width="2.75" customWidth="1"/>
+    <col min="1" max="1" width="2.69921875" style="13" customWidth="1"/>
+    <col min="2" max="2" width="22.69921875" customWidth="1"/>
+    <col min="3" max="3" width="16.69921875" customWidth="1"/>
+    <col min="4" max="4" width="10.69921875" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.69921875" customWidth="1"/>
+    <col min="7" max="7" width="2.69921875" customWidth="1"/>
     <col min="8" max="8" width="6" hidden="1" customWidth="1"/>
-    <col min="9" max="65" width="2.75" customWidth="1"/>
+    <col min="9" max="65" width="2.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="90" customHeight="1">
+    <row r="1" spans="1:64" ht="90" customHeight="1" x14ac:dyDescent="1.45">
       <c r="A1" s="14"/>
-      <c r="B1" s="111" t="s">
+      <c r="B1" s="103" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="18"/>
@@ -1731,31 +1746,31 @@
       <c r="E1" s="20"/>
       <c r="F1" s="21"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="112" t="s">
+      <c r="I1" s="113" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
-      <c r="M1" s="117"/>
-      <c r="N1" s="117"/>
-      <c r="O1" s="117"/>
+      <c r="J1" s="114"/>
+      <c r="K1" s="114"/>
+      <c r="L1" s="114"/>
+      <c r="M1" s="114"/>
+      <c r="N1" s="114"/>
+      <c r="O1" s="114"/>
       <c r="P1" s="24"/>
-      <c r="Q1" s="113">
+      <c r="Q1" s="112">
         <v>45888</v>
       </c>
-      <c r="R1" s="118"/>
-      <c r="S1" s="118"/>
-      <c r="T1" s="118"/>
-      <c r="U1" s="118"/>
-      <c r="V1" s="118"/>
-      <c r="W1" s="118"/>
-      <c r="X1" s="118"/>
-      <c r="Y1" s="118"/>
-      <c r="Z1" s="118"/>
-    </row>
-    <row r="2" spans="1:64" ht="30" customHeight="1">
-      <c r="B2" s="116" t="s">
+      <c r="R1" s="111"/>
+      <c r="S1" s="111"/>
+      <c r="T1" s="111"/>
+      <c r="U1" s="111"/>
+      <c r="V1" s="111"/>
+      <c r="W1" s="111"/>
+      <c r="X1" s="111"/>
+      <c r="Y1" s="111"/>
+      <c r="Z1" s="111"/>
+    </row>
+    <row r="2" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="B2" s="104" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="95"/>
@@ -1765,27 +1780,27 @@
       <c r="I2" s="115" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="119"/>
-      <c r="K2" s="119"/>
-      <c r="L2" s="119"/>
-      <c r="M2" s="119"/>
-      <c r="N2" s="119"/>
-      <c r="O2" s="119"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
       <c r="P2" s="24"/>
-      <c r="Q2" s="114">
+      <c r="Q2" s="110">
         <v>1</v>
       </c>
-      <c r="R2" s="118"/>
-      <c r="S2" s="118"/>
-      <c r="T2" s="118"/>
-      <c r="U2" s="118"/>
-      <c r="V2" s="118"/>
-      <c r="W2" s="118"/>
-      <c r="X2" s="118"/>
-      <c r="Y2" s="118"/>
-      <c r="Z2" s="118"/>
-    </row>
-    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1">
+      <c r="R2" s="111"/>
+      <c r="S2" s="111"/>
+      <c r="T2" s="111"/>
+      <c r="U2" s="111"/>
+      <c r="V2" s="111"/>
+      <c r="W2" s="111"/>
+      <c r="X2" s="111"/>
+      <c r="Y2" s="111"/>
+      <c r="Z2" s="111"/>
+    </row>
+    <row r="3" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="25" t="s">
         <v>4</v>
@@ -1793,106 +1808,106 @@
       <c r="D3" s="27"/>
       <c r="E3" s="28"/>
     </row>
-    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1">
+    <row r="4" spans="1:64" s="26" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="B4" s="29"/>
       <c r="E4" s="30"/>
-      <c r="I4" s="110">
+      <c r="I4" s="107">
         <f>I5</f>
         <v>45887</v>
       </c>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
-      <c r="M4" s="108"/>
-      <c r="N4" s="108"/>
-      <c r="O4" s="108"/>
-      <c r="P4" s="108">
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
+      <c r="P4" s="105">
         <f>P5</f>
         <v>45894</v>
       </c>
-      <c r="Q4" s="108"/>
-      <c r="R4" s="108"/>
-      <c r="S4" s="108"/>
-      <c r="T4" s="108"/>
-      <c r="U4" s="108"/>
-      <c r="V4" s="108"/>
-      <c r="W4" s="108">
+      <c r="Q4" s="105"/>
+      <c r="R4" s="105"/>
+      <c r="S4" s="105"/>
+      <c r="T4" s="105"/>
+      <c r="U4" s="105"/>
+      <c r="V4" s="105"/>
+      <c r="W4" s="105">
         <f>W5</f>
         <v>45901</v>
       </c>
-      <c r="X4" s="108"/>
-      <c r="Y4" s="108"/>
-      <c r="Z4" s="108"/>
-      <c r="AA4" s="108"/>
-      <c r="AB4" s="108"/>
-      <c r="AC4" s="108"/>
-      <c r="AD4" s="108">
+      <c r="X4" s="105"/>
+      <c r="Y4" s="105"/>
+      <c r="Z4" s="105"/>
+      <c r="AA4" s="105"/>
+      <c r="AB4" s="105"/>
+      <c r="AC4" s="105"/>
+      <c r="AD4" s="105">
         <f>AD5</f>
         <v>45908</v>
       </c>
-      <c r="AE4" s="108"/>
-      <c r="AF4" s="108"/>
-      <c r="AG4" s="108"/>
-      <c r="AH4" s="108"/>
-      <c r="AI4" s="108"/>
-      <c r="AJ4" s="108"/>
-      <c r="AK4" s="108">
+      <c r="AE4" s="105"/>
+      <c r="AF4" s="105"/>
+      <c r="AG4" s="105"/>
+      <c r="AH4" s="105"/>
+      <c r="AI4" s="105"/>
+      <c r="AJ4" s="105"/>
+      <c r="AK4" s="105">
         <f>AK5</f>
         <v>45915</v>
       </c>
-      <c r="AL4" s="108"/>
-      <c r="AM4" s="108"/>
-      <c r="AN4" s="108"/>
-      <c r="AO4" s="108"/>
-      <c r="AP4" s="108"/>
-      <c r="AQ4" s="108"/>
-      <c r="AR4" s="108">
+      <c r="AL4" s="105"/>
+      <c r="AM4" s="105"/>
+      <c r="AN4" s="105"/>
+      <c r="AO4" s="105"/>
+      <c r="AP4" s="105"/>
+      <c r="AQ4" s="105"/>
+      <c r="AR4" s="105">
         <f>AR5</f>
         <v>45922</v>
       </c>
-      <c r="AS4" s="108"/>
-      <c r="AT4" s="108"/>
-      <c r="AU4" s="108"/>
-      <c r="AV4" s="108"/>
-      <c r="AW4" s="108"/>
-      <c r="AX4" s="108"/>
-      <c r="AY4" s="108">
+      <c r="AS4" s="105"/>
+      <c r="AT4" s="105"/>
+      <c r="AU4" s="105"/>
+      <c r="AV4" s="105"/>
+      <c r="AW4" s="105"/>
+      <c r="AX4" s="105"/>
+      <c r="AY4" s="105">
         <f>AY5</f>
         <v>45929</v>
       </c>
-      <c r="AZ4" s="108"/>
-      <c r="BA4" s="108"/>
-      <c r="BB4" s="108"/>
-      <c r="BC4" s="108"/>
-      <c r="BD4" s="108"/>
-      <c r="BE4" s="108"/>
-      <c r="BF4" s="108">
+      <c r="AZ4" s="105"/>
+      <c r="BA4" s="105"/>
+      <c r="BB4" s="105"/>
+      <c r="BC4" s="105"/>
+      <c r="BD4" s="105"/>
+      <c r="BE4" s="105"/>
+      <c r="BF4" s="105">
         <f>BF5</f>
         <v>45936</v>
       </c>
-      <c r="BG4" s="108"/>
-      <c r="BH4" s="108"/>
-      <c r="BI4" s="108"/>
-      <c r="BJ4" s="108"/>
-      <c r="BK4" s="108"/>
-      <c r="BL4" s="109"/>
-    </row>
-    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1">
-      <c r="A5" s="103"/>
-      <c r="B5" s="104" t="s">
+      <c r="BG4" s="105"/>
+      <c r="BH4" s="105"/>
+      <c r="BI4" s="105"/>
+      <c r="BJ4" s="105"/>
+      <c r="BK4" s="105"/>
+      <c r="BL4" s="106"/>
+    </row>
+    <row r="5" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="117"/>
+      <c r="B5" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="106" t="s">
+      <c r="C5" s="120" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="107" t="s">
+      <c r="D5" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="107" t="s">
+      <c r="E5" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="107" t="s">
+      <c r="F5" s="108" t="s">
         <v>9</v>
       </c>
       <c r="I5" s="31">
@@ -2120,13 +2135,13 @@
         <v>45942</v>
       </c>
     </row>
-    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="103"/>
-      <c r="B6" s="105"/>
-      <c r="C6" s="120"/>
-      <c r="D6" s="120"/>
-      <c r="E6" s="120"/>
-      <c r="F6" s="120"/>
+    <row r="6" spans="1:64" s="26" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="117"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="109"/>
+      <c r="D6" s="109"/>
+      <c r="E6" s="109"/>
+      <c r="F6" s="109"/>
       <c r="I6" s="34" t="str">
         <f t="shared" ref="I6:AN6" si="3">LEFT(TEXT(I5,"ddd"),1)</f>
         <v>M</v>
@@ -2352,7 +2367,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1">
+    <row r="7" spans="1:64" s="26" customFormat="1" ht="30" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
@@ -2362,7 +2377,7 @@
       <c r="E7" s="37"/>
       <c r="F7" s="37"/>
       <c r="H7" s="26" t="str">
-        <f ca="1">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f>IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I7" s="39"/>
@@ -2422,7 +2437,7 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="8" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="14"/>
       <c r="B8" s="40" t="s">
         <v>11</v>
@@ -2433,7 +2448,7 @@
       <c r="F8" s="44"/>
       <c r="G8" s="17"/>
       <c r="H8" s="5" t="str">
-        <f t="shared" ref="H8:H33" ca="1" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="H8:H33" si="5">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="I8" s="45"/>
@@ -2493,27 +2508,27 @@
       <c r="BK8" s="45"/>
       <c r="BL8" s="45"/>
     </row>
-    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="9" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="47" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="C9" s="48"/>
       <c r="D9" s="49">
         <v>0.5</v>
       </c>
       <c r="E9" s="50">
-        <f>Project_Start</f>
+        <f>J5</f>
         <v>45888</v>
       </c>
       <c r="F9" s="50">
-        <f>E9+3</f>
-        <v>45891</v>
+        <f>E9+14</f>
+        <v>45902</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="5">
-        <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <f t="shared" si="5"/>
+        <v>15</v>
       </c>
       <c r="I9" s="51"/>
       <c r="J9" s="51"/>
@@ -2572,26 +2587,26 @@
       <c r="BK9" s="51"/>
       <c r="BL9" s="51"/>
     </row>
-    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="10" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="47" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="C10" s="52"/>
       <c r="D10" s="53">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="E10" s="54">
-        <f>F9</f>
-        <v>45891</v>
+        <f>S5</f>
+        <v>45897</v>
       </c>
       <c r="F10" s="54">
         <f>E10+2</f>
-        <v>45893</v>
+        <v>45899</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I10" s="51"/>
@@ -2651,27 +2666,27 @@
       <c r="BK10" s="51"/>
       <c r="BL10" s="51"/>
     </row>
-    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="11" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="47" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C11" s="52"/>
       <c r="D11" s="53">
         <v>0.5</v>
       </c>
       <c r="E11" s="54">
-        <f>F10</f>
-        <v>45893</v>
+        <f>J5</f>
+        <v>45888</v>
       </c>
       <c r="F11" s="54">
-        <f>E11+4</f>
+        <f ca="1">TODAY()</f>
         <v>45897</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="5">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I11" s="51"/>
       <c r="J11" s="51"/>
@@ -2730,21 +2745,21 @@
       <c r="BK11" s="51"/>
       <c r="BL11" s="51"/>
     </row>
-    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="12" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="47" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="C12" s="52"/>
       <c r="D12" s="53">
         <v>0.25</v>
       </c>
       <c r="E12" s="54">
-        <f>F11</f>
+        <f ca="1">F11</f>
         <v>45897</v>
       </c>
       <c r="F12" s="54">
-        <f>E12+5</f>
+        <f ca="1">E12+5</f>
         <v>45902</v>
       </c>
       <c r="G12" s="17"/>
@@ -2809,10 +2824,10 @@
       <c r="BK12" s="51"/>
       <c r="BL12" s="51"/>
     </row>
-    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="13" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="47" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="C13" s="52"/>
       <c r="D13" s="53"/>
@@ -2826,7 +2841,7 @@
       </c>
       <c r="G13" s="17"/>
       <c r="H13" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="I13" s="51"/>
@@ -2886,7 +2901,7 @@
       <c r="BK13" s="51"/>
       <c r="BL13" s="51"/>
     </row>
-    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="14" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="56" t="s">
         <v>17</v>
@@ -2897,11 +2912,11 @@
       <c r="F14" s="60"/>
       <c r="G14" s="17"/>
       <c r="H14" s="5" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="15" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="61" t="s">
         <v>12</v>
@@ -2920,7 +2935,7 @@
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I15" s="51"/>
@@ -2980,7 +2995,7 @@
       <c r="BK15" s="51"/>
       <c r="BL15" s="51"/>
     </row>
-    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="16" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="61" t="s">
         <v>13</v>
@@ -2999,7 +3014,7 @@
       </c>
       <c r="G16" s="17"/>
       <c r="H16" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I16" s="51"/>
@@ -3059,7 +3074,7 @@
       <c r="BK16" s="51"/>
       <c r="BL16" s="51"/>
     </row>
-    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="17" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="61" t="s">
         <v>14</v>
@@ -3076,7 +3091,7 @@
       </c>
       <c r="G17" s="17"/>
       <c r="H17" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I17" s="51"/>
@@ -3136,7 +3151,7 @@
       <c r="BK17" s="51"/>
       <c r="BL17" s="51"/>
     </row>
-    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="18" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="61" t="s">
         <v>15</v>
@@ -3153,7 +3168,7 @@
       </c>
       <c r="G18" s="17"/>
       <c r="H18" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="I18" s="51"/>
@@ -3213,7 +3228,7 @@
       <c r="BK18" s="51"/>
       <c r="BL18" s="51"/>
     </row>
-    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="19" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="61" t="s">
         <v>16</v>
@@ -3230,7 +3245,7 @@
       </c>
       <c r="G19" s="17"/>
       <c r="H19" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I19" s="51"/>
@@ -3290,7 +3305,7 @@
       <c r="BK19" s="51"/>
       <c r="BL19" s="51"/>
     </row>
-    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="20" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="65" t="s">
         <v>18</v>
@@ -3301,7 +3316,7 @@
       <c r="F20" s="69"/>
       <c r="G20" s="17"/>
       <c r="H20" s="5" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I20" s="70"/>
@@ -3361,7 +3376,7 @@
       <c r="BK20" s="70"/>
       <c r="BL20" s="70"/>
     </row>
-    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="21" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="71" t="s">
         <v>12</v>
@@ -3380,7 +3395,7 @@
       </c>
       <c r="G21" s="17"/>
       <c r="H21" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I21" s="51"/>
@@ -3440,7 +3455,7 @@
       <c r="BK21" s="51"/>
       <c r="BL21" s="51"/>
     </row>
-    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="22" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="71" t="s">
         <v>13</v>
@@ -3459,7 +3474,7 @@
       </c>
       <c r="G22" s="17"/>
       <c r="H22" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I22" s="51"/>
@@ -3519,7 +3534,7 @@
       <c r="BK22" s="51"/>
       <c r="BL22" s="51"/>
     </row>
-    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="23" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="71" t="s">
         <v>14</v>
@@ -3538,7 +3553,7 @@
       </c>
       <c r="G23" s="17"/>
       <c r="H23" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I23" s="51"/>
@@ -3598,7 +3613,7 @@
       <c r="BK23" s="51"/>
       <c r="BL23" s="51"/>
     </row>
-    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="24" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="71" t="s">
         <v>15</v>
@@ -3617,7 +3632,7 @@
       </c>
       <c r="G24" s="17"/>
       <c r="H24" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I24" s="51"/>
@@ -3677,7 +3692,7 @@
       <c r="BK24" s="51"/>
       <c r="BL24" s="51"/>
     </row>
-    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="25" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="71" t="s">
         <v>16</v>
@@ -3696,7 +3711,7 @@
       </c>
       <c r="G25" s="17"/>
       <c r="H25" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I25" s="51"/>
@@ -3756,7 +3771,7 @@
       <c r="BK25" s="51"/>
       <c r="BL25" s="51"/>
     </row>
-    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="26" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13"/>
       <c r="B26" s="75" t="s">
         <v>19</v>
@@ -3767,7 +3782,7 @@
       <c r="F26" s="79"/>
       <c r="G26" s="17"/>
       <c r="H26" s="5" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I26" s="80"/>
@@ -3827,7 +3842,7 @@
       <c r="BK26" s="80"/>
       <c r="BL26" s="80"/>
     </row>
-    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="27" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13"/>
       <c r="B27" s="81" t="s">
         <v>12</v>
@@ -3846,7 +3861,7 @@
       </c>
       <c r="G27" s="17"/>
       <c r="H27" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I27" s="51"/>
@@ -3906,7 +3921,7 @@
       <c r="BK27" s="51"/>
       <c r="BL27" s="51"/>
     </row>
-    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="28" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13"/>
       <c r="B28" s="81" t="s">
         <v>13</v>
@@ -3925,7 +3940,7 @@
       </c>
       <c r="G28" s="17"/>
       <c r="H28" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="I28" s="51"/>
@@ -3985,7 +4000,7 @@
       <c r="BK28" s="51"/>
       <c r="BL28" s="51"/>
     </row>
-    <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="29" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="13"/>
       <c r="B29" s="81" t="s">
         <v>14</v>
@@ -4004,7 +4019,7 @@
       </c>
       <c r="G29" s="17"/>
       <c r="H29" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I29" s="51"/>
@@ -4064,7 +4079,7 @@
       <c r="BK29" s="51"/>
       <c r="BL29" s="51"/>
     </row>
-    <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="30" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="13"/>
       <c r="B30" s="81" t="s">
         <v>15</v>
@@ -4083,7 +4098,7 @@
       </c>
       <c r="G30" s="17"/>
       <c r="H30" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="I30" s="51"/>
@@ -4143,7 +4158,7 @@
       <c r="BK30" s="51"/>
       <c r="BL30" s="51"/>
     </row>
-    <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="31" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="13"/>
       <c r="B31" s="81" t="s">
         <v>16</v>
@@ -4162,7 +4177,7 @@
       </c>
       <c r="G31" s="17"/>
       <c r="H31" s="5">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="I31" s="51"/>
@@ -4222,7 +4237,7 @@
       <c r="BK31" s="51"/>
       <c r="BL31" s="51"/>
     </row>
-    <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="32" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="13"/>
       <c r="B32" s="85"/>
       <c r="C32" s="86"/>
@@ -4231,7 +4246,7 @@
       <c r="F32" s="88"/>
       <c r="G32" s="17"/>
       <c r="H32" s="5" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I32" s="45"/>
@@ -4291,7 +4306,7 @@
       <c r="BK32" s="45"/>
       <c r="BL32" s="45"/>
     </row>
-    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1">
+    <row r="33" spans="1:64" s="46" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14"/>
       <c r="B33" s="89" t="s">
         <v>20</v>
@@ -4302,7 +4317,7 @@
       <c r="F33" s="93"/>
       <c r="G33" s="17"/>
       <c r="H33" s="6" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I33" s="94"/>
@@ -4362,18 +4377,28 @@
       <c r="BK33" s="94"/>
       <c r="BL33" s="94"/>
     </row>
-    <row r="34" spans="1:64" ht="30" customHeight="1">
+    <row r="34" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:64" ht="30" customHeight="1">
+    <row r="35" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C35" s="16"/>
       <c r="F35" s="15"/>
     </row>
-    <row r="36" spans="1:64" ht="30" customHeight="1">
+    <row r="36" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="Q2:Z2"/>
+    <mergeCell ref="Q1:Z1"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="I2:O2"/>
     <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
@@ -4382,16 +4407,6 @@
     <mergeCell ref="AK4:AQ4"/>
     <mergeCell ref="AR4:AX4"/>
     <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="Q2:Z2"/>
-    <mergeCell ref="Q1:Z1"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="I2:O2"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D33">
     <cfRule type="dataBar" priority="23">
@@ -4407,41 +4422,41 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I4:BL31">
+    <cfRule type="expression" dxfId="8" priority="1">
+      <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="I9:BL13">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15:BL19">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="5" priority="4">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="5" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21:BL25">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I27:BL31">
-    <cfRule type="expression" dxfId="2" priority="36">
+    <cfRule type="expression" dxfId="1" priority="36">
       <formula>AND(task_start&lt;=I$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=I$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="37" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="37" stopIfTrue="1">
       <formula>AND(task_end&gt;=I$5,task_start&lt;J$5)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:BL31 I21:BL25 I15:BL19 I9:BL13 I27:BL31">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>AND(TODAY()&gt;=I$5, TODAY()&lt;J$5)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="13">
@@ -4500,110 +4515,110 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="87" style="7" customWidth="1"/>
     <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="46.5" customHeight="1"/>
-    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.6">
+    <row r="1" spans="1:2" ht="46.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" s="9" customFormat="1" ht="15.6" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="8"/>
     </row>
-    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1">
+    <row r="3" spans="1:2" s="11" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="97"/>
       <c r="B3" s="12"/>
     </row>
-    <row r="4" spans="1:2" s="10" customFormat="1" ht="30">
+    <row r="4" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A4" s="98" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="74.25" customHeight="1">
+    <row r="5" spans="1:2" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="99" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" customHeight="1">
+    <row r="6" spans="1:2" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="98" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.15" customHeight="1">
+    <row r="7" spans="1:2" s="7" customFormat="1" ht="205.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="100" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="10" customFormat="1" ht="30">
+    <row r="8" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A8" s="98" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="41.45">
+    <row r="9" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="99" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1">
+    <row r="10" spans="1:2" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="101" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" s="10" customFormat="1" ht="30">
+    <row r="11" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A11" s="98" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="27.6">
+    <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A12" s="99" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.15" customHeight="1">
+    <row r="13" spans="1:2" s="7" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="101" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:2" s="10" customFormat="1" ht="30">
+    <row r="14" spans="1:2" s="10" customFormat="1" ht="30" x14ac:dyDescent="0.7">
       <c r="A14" s="98" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="75" customHeight="1">
+    <row r="15" spans="1:2" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="99" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="69">
+    <row r="16" spans="1:2" ht="69" x14ac:dyDescent="0.25">
       <c r="A16" s="99" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="102"/>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="102"/>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="102"/>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="102"/>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="102"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="102"/>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="102"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="102"/>
     </row>
   </sheetData>
@@ -4619,12 +4634,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4940,35 +4966,53 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2348D59-3426-404A-A0C5-6456F6613EDB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A82239A0-E68C-493F-BEE6-C77FEA397FD6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97245281-08F3-4104-84BD-39F3D8CFB195}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>